<commit_message>
update Project, Suite,Section and TestCase IDs, also the xml data file.  Test pass but Failed to when write to TestRail
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData-seleniumframework.xlsx
+++ b/src/test/resources/testData/TestData-seleniumframework.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
@@ -11,12 +11,12 @@
     <sheet name="SignInContactUs" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="21">
   <si>
     <t>Test Case Name</t>
   </si>
@@ -60,29 +60,32 @@
     <t>Customer service</t>
   </si>
   <si>
-    <t>abc@123.com</t>
-  </si>
-  <si>
     <t>Testmessage1</t>
   </si>
   <si>
     <t>Testmessage2</t>
   </si>
   <si>
-    <t>abc@234.com</t>
-  </si>
-  <si>
     <t>abc123</t>
   </si>
   <si>
     <t>bcd234</t>
+  </si>
+  <si>
+    <t>alistair.zhu@laserfiche.com</t>
+  </si>
+  <si>
+    <t>19Unipas91</t>
+  </si>
+  <si>
+    <t>testcase-001</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -172,6 +175,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -219,7 +225,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -251,9 +257,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -285,6 +292,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -460,14 +468,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M3"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
       <selection sqref="A1:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="17.7109375" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -481,7 +489,7 @@
     <col min="13" max="13" width="20" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" customHeight="1">
+    <row r="1" spans="1:4" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -495,7 +503,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -509,7 +517,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -536,25 +544,25 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" style="6" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.140625" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" customWidth="1"/>
+    <col min="6" max="6" width="33.140625" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="6" customWidth="1"/>
+    <col min="8" max="8" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="30" customHeight="1">
+    <row r="1" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -580,15 +588,15 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>6</v>
@@ -597,24 +605,24 @@
         <v>13</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="5" t="s">
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>4</v>
-      </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>6</v>
@@ -623,21 +631,21 @@
         <v>13</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="5" t="s">
-        <v>19</v>
-      </c>
       <c r="H3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>
-    <hyperlink ref="C3" r:id="rId3"/>
-    <hyperlink ref="C2" r:id="rId4"/>
+    <hyperlink ref="C3" r:id="rId3" display="Test@123"/>
+    <hyperlink ref="C2" r:id="rId4" display="Test@123"/>
     <hyperlink ref="F2" r:id="rId5"/>
     <hyperlink ref="F3" r:id="rId6"/>
   </hyperlinks>
@@ -646,12 +654,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>